<commit_message>
Add stats and outputs
</commit_message>
<xml_diff>
--- a/out/stats/potential_neg_overall_hoho_stats.xlsx
+++ b/out/stats/potential_neg_overall_hoho_stats.xlsx
@@ -552,7 +552,7 @@
         <v>-544.0769230769231</v>
       </c>
       <c r="C3">
-        <v>-1314.457975806451</v>
+        <v>-1314.457975806452</v>
       </c>
       <c r="D3">
         <v>-1353.046181818182</v>
@@ -564,7 +564,7 @@
         <v>-1243.5834375</v>
       </c>
       <c r="G3">
-        <v>-598.0322972972972</v>
+        <v>-598.0322972972973</v>
       </c>
       <c r="H3">
         <v>-3015.238095238095</v>
@@ -573,7 +573,7 @@
         <v>-792</v>
       </c>
       <c r="J3">
-        <v>-3459.475707317073</v>
+        <v>-3459.475707317074</v>
       </c>
       <c r="K3">
         <v>-318.1538461538461</v>
@@ -599,10 +599,10 @@
         <v>1285.020998898982</v>
       </c>
       <c r="C4">
-        <v>2817.552337000042</v>
+        <v>2817.552337000043</v>
       </c>
       <c r="D4">
-        <v>3888.884159811794</v>
+        <v>3888.884159811795</v>
       </c>
       <c r="E4">
         <v>4101.53918404468</v>
@@ -620,7 +620,7 @@
         <v>266.6833328125326</v>
       </c>
       <c r="J4">
-        <v>6611.25953580335</v>
+        <v>6611.259535803349</v>
       </c>
       <c r="K4">
         <v>733.3886934692285</v>
@@ -1379,7 +1379,7 @@
         <v>-675.5948794444444</v>
       </c>
       <c r="G3">
-        <v>-2835.928062068966</v>
+        <v>-2835.928062068965</v>
       </c>
       <c r="H3">
         <v>-207.3448275862069</v>
@@ -1423,7 +1423,7 @@
         <v>225.3473900809763</v>
       </c>
       <c r="J4">
-        <v>705.7571961803793</v>
+        <v>705.7571961803792</v>
       </c>
       <c r="K4">
         <v>457.8953246470603</v>
@@ -1763,7 +1763,7 @@
         <v>2688.916002116197</v>
       </c>
       <c r="I4">
-        <v>2354.651050368282</v>
+        <v>2354.651050368283</v>
       </c>
       <c r="J4">
         <v>85.10063587659604</v>
@@ -2402,7 +2402,7 @@
         <v>-552.0104502777779</v>
       </c>
       <c r="E3">
-        <v>-4717.517599999999</v>
+        <v>-4717.5176</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2414,7 +2414,7 @@
         <v>-1150.223262222222</v>
       </c>
       <c r="I3">
-        <v>-483.6250249999999</v>
+        <v>-483.625025</v>
       </c>
       <c r="J3">
         <v>-1208.656838888889</v>
@@ -2449,10 +2449,10 @@
         <v>1463.839619186687</v>
       </c>
       <c r="I4">
-        <v>545.7855650461599</v>
+        <v>545.7855650461598</v>
       </c>
       <c r="J4">
-        <v>938.4671061325388</v>
+        <v>938.4671061325387</v>
       </c>
       <c r="K4">
         <v>360.7638458618059</v>
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>-527.2935644444445</v>
+        <v>-527.2935644444444</v>
       </c>
       <c r="E3">
         <v>-5576.188566666667</v>
@@ -3049,7 +3049,7 @@
         <v>-469.8544700892858</v>
       </c>
       <c r="D3">
-        <v>-350.6212253333334</v>
+        <v>-350.6212253333333</v>
       </c>
       <c r="E3">
         <v>-514.3095134821427</v>
@@ -3078,7 +3078,7 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>7592.099153479998</v>
+        <v>7592.099153479999</v>
       </c>
       <c r="C4">
         <v>526.7631714057043</v>

</xml_diff>